<commit_message>
upload develop branch. add results files for LLM, REACH, and INDRA. enable more attributes to be compared. order of entity match - hgnc > name > id. Regulate model's .
</commit_message>
<xml_diff>
--- a/examples/input/interactions/INDRA/RA4_reading_BioRECIPE.xlsx
+++ b/examples/input/interactions/INDRA/RA4_reading_BioRECIPE.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jasmine/Desktop/violin_org/VIOLIN/examples/new_reading_input/INDRA/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jasmine/Desktop/github_local_copy/VIOLIN/examples/input/interactions/INDRA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0E35CB1-9A4E-D745-93C5-0EF5E9A671AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BDEE853-458B-CF4C-9D06-7282F78FB719}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2100" yWindow="6360" windowWidth="38400" windowHeight="20100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8240" yWindow="1480" windowWidth="38400" windowHeight="20100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,9 +31,6 @@
     <t>Regulator Subtype</t>
   </si>
   <si>
-    <t>Regulator HGNC ID</t>
-  </si>
-  <si>
     <t>Regulator Database</t>
   </si>
   <si>
@@ -55,9 +52,6 @@
     <t>Regulated Subtype</t>
   </si>
   <si>
-    <t>Regulated HGNC ID</t>
-  </si>
-  <si>
     <t>Regulated Database</t>
   </si>
   <si>
@@ -434,6 +428,12 @@
   </si>
   <si>
     <t>Ltn1 ubiquitylates TYW3 and RSK1/2 in a regulatory manner.</t>
+  </si>
+  <si>
+    <t>Regulator HGNC Symbol</t>
+  </si>
+  <si>
+    <t>Regulated HGNC Symbol</t>
   </si>
 </sst>
 </file>
@@ -451,8 +451,10 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -800,7 +802,7 @@
   <dimension ref="A1:AB31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -816,1420 +818,1420 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>25</v>
-      </c>
-      <c r="AA1" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="AB1" s="1" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" t="s">
         <v>28</v>
       </c>
-      <c r="B2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F2" t="s">
         <v>30</v>
       </c>
-      <c r="E2" t="s">
+      <c r="I2" t="s">
         <v>31</v>
       </c>
-      <c r="F2" t="s">
+      <c r="J2" t="s">
         <v>32</v>
       </c>
-      <c r="I2" t="s">
+      <c r="M2" t="s">
         <v>33</v>
       </c>
-      <c r="J2" t="s">
+      <c r="N2" t="s">
         <v>34</v>
       </c>
-      <c r="M2" t="s">
+      <c r="Q2" t="s">
         <v>35</v>
       </c>
-      <c r="N2" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q2" t="s">
+      <c r="R2" t="s">
+        <v>36</v>
+      </c>
+      <c r="S2" t="s">
         <v>37</v>
       </c>
-      <c r="R2" t="s">
+      <c r="Y2">
+        <v>0.65</v>
+      </c>
+      <c r="AA2" t="s">
         <v>38</v>
       </c>
-      <c r="S2" t="s">
+      <c r="AB2" t="s">
         <v>39</v>
-      </c>
-      <c r="Y2">
-        <v>0.65</v>
-      </c>
-      <c r="AA2" t="s">
-        <v>40</v>
-      </c>
-      <c r="AB2" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F3" t="s">
+        <v>40</v>
+      </c>
+      <c r="I3" t="s">
         <v>43</v>
       </c>
-      <c r="E3" t="s">
+      <c r="J3" t="s">
+        <v>27</v>
+      </c>
+      <c r="L3" t="s">
         <v>44</v>
       </c>
-      <c r="F3" t="s">
-        <v>42</v>
-      </c>
-      <c r="I3" t="s">
+      <c r="M3" t="s">
+        <v>29</v>
+      </c>
+      <c r="N3" t="s">
         <v>45</v>
       </c>
-      <c r="J3" t="s">
-        <v>29</v>
-      </c>
-      <c r="L3" t="s">
+      <c r="Q3" t="s">
+        <v>35</v>
+      </c>
+      <c r="R3" t="s">
+        <v>36</v>
+      </c>
+      <c r="S3" t="s">
+        <v>37</v>
+      </c>
+      <c r="Y3">
+        <v>0.65</v>
+      </c>
+      <c r="AA3" t="s">
         <v>46</v>
       </c>
-      <c r="M3" t="s">
-        <v>31</v>
-      </c>
-      <c r="N3" t="s">
-        <v>47</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>37</v>
-      </c>
-      <c r="R3" t="s">
-        <v>38</v>
-      </c>
-      <c r="S3" t="s">
+      <c r="AB3" t="s">
         <v>39</v>
-      </c>
-      <c r="Y3">
-        <v>0.65</v>
-      </c>
-      <c r="AA3" t="s">
-        <v>48</v>
-      </c>
-      <c r="AB3" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B4" t="s">
+        <v>41</v>
+      </c>
+      <c r="E4" t="s">
+        <v>42</v>
+      </c>
+      <c r="F4" t="s">
+        <v>47</v>
+      </c>
+      <c r="I4" t="s">
+        <v>48</v>
+      </c>
+      <c r="J4" t="s">
+        <v>27</v>
+      </c>
+      <c r="L4" t="s">
         <v>49</v>
       </c>
-      <c r="B4" t="s">
-        <v>43</v>
-      </c>
-      <c r="E4" t="s">
-        <v>44</v>
-      </c>
-      <c r="F4" t="s">
-        <v>49</v>
-      </c>
-      <c r="I4" t="s">
+      <c r="M4" t="s">
+        <v>29</v>
+      </c>
+      <c r="N4" t="s">
         <v>50</v>
       </c>
-      <c r="J4" t="s">
-        <v>29</v>
-      </c>
-      <c r="L4" t="s">
+      <c r="Q4" t="s">
+        <v>35</v>
+      </c>
+      <c r="R4" t="s">
+        <v>36</v>
+      </c>
+      <c r="S4" t="s">
+        <v>37</v>
+      </c>
+      <c r="Y4">
+        <v>0.65</v>
+      </c>
+      <c r="AA4" t="s">
         <v>51</v>
       </c>
-      <c r="M4" t="s">
-        <v>31</v>
-      </c>
-      <c r="N4" t="s">
-        <v>52</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>37</v>
-      </c>
-      <c r="R4" t="s">
-        <v>38</v>
-      </c>
-      <c r="S4" t="s">
+      <c r="AB4" t="s">
         <v>39</v>
-      </c>
-      <c r="Y4">
-        <v>0.65</v>
-      </c>
-      <c r="AA4" t="s">
-        <v>53</v>
-      </c>
-      <c r="AB4" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B5" t="s">
+        <v>53</v>
+      </c>
+      <c r="E5" t="s">
         <v>54</v>
       </c>
-      <c r="B5" t="s">
+      <c r="F5" t="s">
         <v>55</v>
       </c>
-      <c r="E5" t="s">
-        <v>56</v>
-      </c>
-      <c r="F5" t="s">
-        <v>57</v>
-      </c>
       <c r="I5" t="s">
+        <v>43</v>
+      </c>
+      <c r="J5" t="s">
+        <v>27</v>
+      </c>
+      <c r="L5" t="s">
+        <v>44</v>
+      </c>
+      <c r="M5" t="s">
+        <v>29</v>
+      </c>
+      <c r="N5" t="s">
         <v>45</v>
       </c>
-      <c r="J5" t="s">
-        <v>29</v>
-      </c>
-      <c r="L5" t="s">
+      <c r="Q5" t="s">
+        <v>35</v>
+      </c>
+      <c r="R5" t="s">
+        <v>36</v>
+      </c>
+      <c r="S5" t="s">
+        <v>37</v>
+      </c>
+      <c r="Y5">
+        <v>0.65</v>
+      </c>
+      <c r="AA5" t="s">
         <v>46</v>
       </c>
-      <c r="M5" t="s">
-        <v>31</v>
-      </c>
-      <c r="N5" t="s">
-        <v>47</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>37</v>
-      </c>
-      <c r="R5" t="s">
-        <v>38</v>
-      </c>
-      <c r="S5" t="s">
+      <c r="AB5" t="s">
         <v>39</v>
-      </c>
-      <c r="Y5">
-        <v>0.65</v>
-      </c>
-      <c r="AA5" t="s">
-        <v>48</v>
-      </c>
-      <c r="AB5" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>56</v>
+      </c>
+      <c r="B6" t="s">
+        <v>41</v>
+      </c>
+      <c r="E6" t="s">
+        <v>42</v>
+      </c>
+      <c r="F6" t="s">
+        <v>56</v>
+      </c>
+      <c r="I6" t="s">
+        <v>57</v>
+      </c>
+      <c r="J6" t="s">
+        <v>27</v>
+      </c>
+      <c r="L6" t="s">
         <v>58</v>
       </c>
-      <c r="B6" t="s">
-        <v>43</v>
-      </c>
-      <c r="E6" t="s">
-        <v>44</v>
-      </c>
-      <c r="F6" t="s">
-        <v>58</v>
-      </c>
-      <c r="I6" t="s">
+      <c r="M6" t="s">
+        <v>29</v>
+      </c>
+      <c r="N6" t="s">
         <v>59</v>
       </c>
-      <c r="J6" t="s">
-        <v>29</v>
-      </c>
-      <c r="L6" t="s">
+      <c r="Q6" t="s">
+        <v>35</v>
+      </c>
+      <c r="R6" t="s">
+        <v>36</v>
+      </c>
+      <c r="S6" t="s">
+        <v>37</v>
+      </c>
+      <c r="Y6">
+        <v>0.65</v>
+      </c>
+      <c r="AA6" t="s">
         <v>60</v>
       </c>
-      <c r="M6" t="s">
-        <v>31</v>
-      </c>
-      <c r="N6" t="s">
+      <c r="AB6" t="s">
         <v>61</v>
-      </c>
-      <c r="Q6" t="s">
-        <v>37</v>
-      </c>
-      <c r="R6" t="s">
-        <v>38</v>
-      </c>
-      <c r="S6" t="s">
-        <v>39</v>
-      </c>
-      <c r="Y6">
-        <v>0.65</v>
-      </c>
-      <c r="AA6" t="s">
-        <v>62</v>
-      </c>
-      <c r="AB6" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="7" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>62</v>
+      </c>
+      <c r="B7" t="s">
+        <v>41</v>
+      </c>
+      <c r="E7" t="s">
+        <v>42</v>
+      </c>
+      <c r="F7" t="s">
+        <v>62</v>
+      </c>
+      <c r="I7" t="s">
+        <v>63</v>
+      </c>
+      <c r="J7" t="s">
+        <v>27</v>
+      </c>
+      <c r="L7" t="s">
         <v>64</v>
       </c>
-      <c r="B7" t="s">
-        <v>43</v>
-      </c>
-      <c r="E7" t="s">
-        <v>44</v>
-      </c>
-      <c r="F7" t="s">
-        <v>64</v>
-      </c>
-      <c r="I7" t="s">
+      <c r="M7" t="s">
+        <v>29</v>
+      </c>
+      <c r="N7" t="s">
         <v>65</v>
       </c>
-      <c r="J7" t="s">
-        <v>29</v>
-      </c>
-      <c r="L7" t="s">
+      <c r="Q7" t="s">
+        <v>35</v>
+      </c>
+      <c r="R7" t="s">
+        <v>36</v>
+      </c>
+      <c r="S7" t="s">
+        <v>37</v>
+      </c>
+      <c r="Y7">
+        <v>0.65</v>
+      </c>
+      <c r="AA7" t="s">
         <v>66</v>
       </c>
-      <c r="M7" t="s">
-        <v>31</v>
-      </c>
-      <c r="N7" t="s">
-        <v>67</v>
-      </c>
-      <c r="Q7" t="s">
-        <v>37</v>
-      </c>
-      <c r="R7" t="s">
-        <v>38</v>
-      </c>
-      <c r="S7" t="s">
-        <v>39</v>
-      </c>
-      <c r="Y7">
-        <v>0.65</v>
-      </c>
-      <c r="AA7" t="s">
-        <v>68</v>
-      </c>
       <c r="AB7" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="8" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
+        <v>57</v>
+      </c>
+      <c r="B8" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" t="s">
+        <v>58</v>
+      </c>
+      <c r="E8" t="s">
+        <v>29</v>
+      </c>
+      <c r="F8" t="s">
         <v>59</v>
       </c>
-      <c r="B8" t="s">
-        <v>29</v>
-      </c>
-      <c r="D8" t="s">
-        <v>60</v>
-      </c>
-      <c r="E8" t="s">
-        <v>31</v>
-      </c>
-      <c r="F8" t="s">
+      <c r="I8" t="s">
+        <v>67</v>
+      </c>
+      <c r="J8" t="s">
+        <v>53</v>
+      </c>
+      <c r="M8" t="s">
+        <v>54</v>
+      </c>
+      <c r="N8" t="s">
+        <v>68</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>35</v>
+      </c>
+      <c r="R8" t="s">
+        <v>36</v>
+      </c>
+      <c r="S8" t="s">
+        <v>37</v>
+      </c>
+      <c r="Y8">
+        <v>0.65</v>
+      </c>
+      <c r="AA8" t="s">
+        <v>69</v>
+      </c>
+      <c r="AB8" t="s">
         <v>61</v>
-      </c>
-      <c r="I8" t="s">
-        <v>69</v>
-      </c>
-      <c r="J8" t="s">
-        <v>55</v>
-      </c>
-      <c r="M8" t="s">
-        <v>56</v>
-      </c>
-      <c r="N8" t="s">
-        <v>70</v>
-      </c>
-      <c r="Q8" t="s">
-        <v>37</v>
-      </c>
-      <c r="R8" t="s">
-        <v>38</v>
-      </c>
-      <c r="S8" t="s">
-        <v>39</v>
-      </c>
-      <c r="Y8">
-        <v>0.65</v>
-      </c>
-      <c r="AA8" t="s">
-        <v>71</v>
-      </c>
-      <c r="AB8" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="9" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B9" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E9" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F9" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="I9" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="J9" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="M9" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="N9" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="Q9" t="s">
+        <v>35</v>
+      </c>
+      <c r="R9" t="s">
+        <v>36</v>
+      </c>
+      <c r="S9" t="s">
         <v>37</v>
       </c>
-      <c r="R9" t="s">
-        <v>38</v>
-      </c>
-      <c r="S9" t="s">
-        <v>39</v>
-      </c>
       <c r="Y9">
         <v>0.65</v>
       </c>
       <c r="AA9" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="AB9" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="10" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
+        <v>72</v>
+      </c>
+      <c r="B10" t="s">
+        <v>27</v>
+      </c>
+      <c r="D10" t="s">
+        <v>73</v>
+      </c>
+      <c r="E10" t="s">
+        <v>29</v>
+      </c>
+      <c r="F10" t="s">
         <v>74</v>
       </c>
-      <c r="B10" t="s">
-        <v>29</v>
-      </c>
-      <c r="D10" t="s">
+      <c r="I10" t="s">
         <v>75</v>
       </c>
-      <c r="E10" t="s">
-        <v>31</v>
-      </c>
-      <c r="F10" t="s">
+      <c r="J10" t="s">
+        <v>41</v>
+      </c>
+      <c r="M10" t="s">
+        <v>42</v>
+      </c>
+      <c r="N10" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>35</v>
+      </c>
+      <c r="R10" t="s">
+        <v>36</v>
+      </c>
+      <c r="S10" t="s">
+        <v>37</v>
+      </c>
+      <c r="Y10">
+        <v>0.65</v>
+      </c>
+      <c r="AA10" t="s">
         <v>76</v>
       </c>
-      <c r="I10" t="s">
+      <c r="AB10" t="s">
         <v>77</v>
-      </c>
-      <c r="J10" t="s">
-        <v>43</v>
-      </c>
-      <c r="M10" t="s">
-        <v>44</v>
-      </c>
-      <c r="N10" t="s">
-        <v>77</v>
-      </c>
-      <c r="Q10" t="s">
-        <v>37</v>
-      </c>
-      <c r="R10" t="s">
-        <v>38</v>
-      </c>
-      <c r="S10" t="s">
-        <v>39</v>
-      </c>
-      <c r="Y10">
-        <v>0.65</v>
-      </c>
-      <c r="AA10" t="s">
-        <v>78</v>
-      </c>
-      <c r="AB10" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="11" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
+        <v>78</v>
+      </c>
+      <c r="B11" t="s">
+        <v>41</v>
+      </c>
+      <c r="E11" t="s">
+        <v>42</v>
+      </c>
+      <c r="F11" t="s">
+        <v>78</v>
+      </c>
+      <c r="I11" t="s">
+        <v>79</v>
+      </c>
+      <c r="J11" t="s">
+        <v>27</v>
+      </c>
+      <c r="L11" t="s">
         <v>80</v>
       </c>
-      <c r="B11" t="s">
-        <v>43</v>
-      </c>
-      <c r="E11" t="s">
-        <v>44</v>
-      </c>
-      <c r="F11" t="s">
-        <v>80</v>
-      </c>
-      <c r="I11" t="s">
+      <c r="M11" t="s">
+        <v>29</v>
+      </c>
+      <c r="N11" t="s">
         <v>81</v>
       </c>
-      <c r="J11" t="s">
-        <v>29</v>
-      </c>
-      <c r="L11" t="s">
+      <c r="R11" t="s">
+        <v>36</v>
+      </c>
+      <c r="S11" t="s">
         <v>82</v>
       </c>
-      <c r="M11" t="s">
-        <v>31</v>
-      </c>
-      <c r="N11" t="s">
+      <c r="Y11">
+        <v>0.65</v>
+      </c>
+      <c r="AA11" t="s">
         <v>83</v>
       </c>
-      <c r="R11" t="s">
-        <v>38</v>
-      </c>
-      <c r="S11" t="s">
-        <v>84</v>
-      </c>
-      <c r="Y11">
-        <v>0.65</v>
-      </c>
-      <c r="AA11" t="s">
-        <v>85</v>
-      </c>
       <c r="AB11" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="12" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B12" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E12" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F12" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="I12" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="J12" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="M12" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="N12" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="R12" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="S12" t="s">
+        <v>82</v>
+      </c>
+      <c r="Y12">
+        <v>0.65</v>
+      </c>
+      <c r="AA12" t="s">
         <v>84</v>
       </c>
-      <c r="Y12">
-        <v>0.65</v>
-      </c>
-      <c r="AA12" t="s">
-        <v>86</v>
-      </c>
       <c r="AB12" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="13" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
+        <v>85</v>
+      </c>
+      <c r="B13" t="s">
+        <v>41</v>
+      </c>
+      <c r="E13" t="s">
+        <v>42</v>
+      </c>
+      <c r="F13" t="s">
+        <v>85</v>
+      </c>
+      <c r="I13" t="s">
+        <v>86</v>
+      </c>
+      <c r="J13" t="s">
+        <v>27</v>
+      </c>
+      <c r="L13" t="s">
         <v>87</v>
       </c>
-      <c r="B13" t="s">
-        <v>43</v>
-      </c>
-      <c r="E13" t="s">
-        <v>44</v>
-      </c>
-      <c r="F13" t="s">
-        <v>87</v>
-      </c>
-      <c r="I13" t="s">
+      <c r="M13" t="s">
+        <v>29</v>
+      </c>
+      <c r="N13" t="s">
         <v>88</v>
       </c>
-      <c r="J13" t="s">
-        <v>29</v>
-      </c>
-      <c r="L13" t="s">
+      <c r="R13" t="s">
+        <v>36</v>
+      </c>
+      <c r="S13" t="s">
+        <v>82</v>
+      </c>
+      <c r="Y13">
+        <v>0.65</v>
+      </c>
+      <c r="AA13" t="s">
         <v>89</v>
       </c>
-      <c r="M13" t="s">
-        <v>31</v>
-      </c>
-      <c r="N13" t="s">
-        <v>90</v>
-      </c>
-      <c r="R13" t="s">
-        <v>38</v>
-      </c>
-      <c r="S13" t="s">
-        <v>84</v>
-      </c>
-      <c r="Y13">
-        <v>0.65</v>
-      </c>
-      <c r="AA13" t="s">
-        <v>91</v>
-      </c>
       <c r="AB13" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="14" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
+        <v>90</v>
+      </c>
+      <c r="B14" t="s">
+        <v>53</v>
+      </c>
+      <c r="E14" t="s">
+        <v>54</v>
+      </c>
+      <c r="F14" t="s">
+        <v>91</v>
+      </c>
+      <c r="I14" t="s">
         <v>92</v>
       </c>
-      <c r="B14" t="s">
-        <v>55</v>
-      </c>
-      <c r="E14" t="s">
-        <v>56</v>
-      </c>
-      <c r="F14" t="s">
+      <c r="J14" t="s">
+        <v>27</v>
+      </c>
+      <c r="L14" t="s">
         <v>93</v>
       </c>
-      <c r="I14" t="s">
+      <c r="M14" t="s">
+        <v>29</v>
+      </c>
+      <c r="N14" t="s">
         <v>94</v>
       </c>
-      <c r="J14" t="s">
-        <v>29</v>
-      </c>
-      <c r="L14" t="s">
+      <c r="R14" t="s">
+        <v>36</v>
+      </c>
+      <c r="S14" t="s">
+        <v>82</v>
+      </c>
+      <c r="Y14">
+        <v>0.65</v>
+      </c>
+      <c r="AA14" t="s">
         <v>95</v>
       </c>
-      <c r="M14" t="s">
-        <v>31</v>
-      </c>
-      <c r="N14" t="s">
-        <v>96</v>
-      </c>
-      <c r="R14" t="s">
-        <v>38</v>
-      </c>
-      <c r="S14" t="s">
-        <v>84</v>
-      </c>
-      <c r="Y14">
-        <v>0.65</v>
-      </c>
-      <c r="AA14" t="s">
-        <v>97</v>
-      </c>
       <c r="AB14" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="15" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B15" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E15" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F15" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="I15" t="s">
+        <v>92</v>
+      </c>
+      <c r="J15" t="s">
+        <v>27</v>
+      </c>
+      <c r="L15" t="s">
+        <v>93</v>
+      </c>
+      <c r="M15" t="s">
+        <v>29</v>
+      </c>
+      <c r="N15" t="s">
         <v>94</v>
       </c>
-      <c r="J15" t="s">
-        <v>29</v>
-      </c>
-      <c r="L15" t="s">
-        <v>95</v>
-      </c>
-      <c r="M15" t="s">
-        <v>31</v>
-      </c>
-      <c r="N15" t="s">
-        <v>96</v>
-      </c>
       <c r="R15" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="S15" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="Y15">
         <v>0.65</v>
       </c>
       <c r="AA15" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="AB15" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="16" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
+        <v>98</v>
+      </c>
+      <c r="B16" t="s">
+        <v>41</v>
+      </c>
+      <c r="E16" t="s">
+        <v>42</v>
+      </c>
+      <c r="F16" t="s">
+        <v>98</v>
+      </c>
+      <c r="I16" t="s">
+        <v>99</v>
+      </c>
+      <c r="J16" t="s">
+        <v>41</v>
+      </c>
+      <c r="M16" t="s">
+        <v>42</v>
+      </c>
+      <c r="N16" t="s">
+        <v>99</v>
+      </c>
+      <c r="Q16" t="s">
         <v>100</v>
       </c>
-      <c r="B16" t="s">
-        <v>43</v>
-      </c>
-      <c r="E16" t="s">
-        <v>44</v>
-      </c>
-      <c r="F16" t="s">
-        <v>100</v>
-      </c>
-      <c r="I16" t="s">
+      <c r="R16" t="s">
+        <v>36</v>
+      </c>
+      <c r="S16" t="s">
         <v>101</v>
       </c>
-      <c r="J16" t="s">
-        <v>43</v>
-      </c>
-      <c r="M16" t="s">
-        <v>44</v>
-      </c>
-      <c r="N16" t="s">
-        <v>101</v>
-      </c>
-      <c r="Q16" t="s">
-        <v>102</v>
-      </c>
-      <c r="R16" t="s">
-        <v>38</v>
-      </c>
-      <c r="S16" t="s">
-        <v>103</v>
-      </c>
       <c r="Y16">
         <v>0.65</v>
       </c>
       <c r="AA16" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="AB16" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="17" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
+        <v>98</v>
+      </c>
+      <c r="B17" t="s">
+        <v>41</v>
+      </c>
+      <c r="E17" t="s">
+        <v>42</v>
+      </c>
+      <c r="F17" t="s">
+        <v>98</v>
+      </c>
+      <c r="I17" t="s">
+        <v>102</v>
+      </c>
+      <c r="J17" t="s">
+        <v>41</v>
+      </c>
+      <c r="M17" t="s">
+        <v>42</v>
+      </c>
+      <c r="N17" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q17" t="s">
         <v>100</v>
       </c>
-      <c r="B17" t="s">
-        <v>43</v>
-      </c>
-      <c r="E17" t="s">
-        <v>44</v>
-      </c>
-      <c r="F17" t="s">
-        <v>100</v>
-      </c>
-      <c r="I17" t="s">
-        <v>104</v>
-      </c>
-      <c r="J17" t="s">
-        <v>43</v>
-      </c>
-      <c r="M17" t="s">
-        <v>44</v>
-      </c>
-      <c r="N17" t="s">
-        <v>104</v>
-      </c>
-      <c r="Q17" t="s">
-        <v>102</v>
-      </c>
       <c r="R17" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="S17" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="Y17">
         <v>0.65</v>
       </c>
       <c r="AA17" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="AB17" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="18" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
+        <v>98</v>
+      </c>
+      <c r="B18" t="s">
+        <v>41</v>
+      </c>
+      <c r="E18" t="s">
+        <v>42</v>
+      </c>
+      <c r="F18" t="s">
+        <v>98</v>
+      </c>
+      <c r="I18" t="s">
+        <v>103</v>
+      </c>
+      <c r="J18" t="s">
+        <v>41</v>
+      </c>
+      <c r="M18" t="s">
+        <v>42</v>
+      </c>
+      <c r="N18" t="s">
+        <v>103</v>
+      </c>
+      <c r="Q18" t="s">
         <v>100</v>
       </c>
-      <c r="B18" t="s">
-        <v>43</v>
-      </c>
-      <c r="E18" t="s">
-        <v>44</v>
-      </c>
-      <c r="F18" t="s">
-        <v>100</v>
-      </c>
-      <c r="I18" t="s">
-        <v>105</v>
-      </c>
-      <c r="J18" t="s">
-        <v>43</v>
-      </c>
-      <c r="M18" t="s">
-        <v>44</v>
-      </c>
-      <c r="N18" t="s">
-        <v>105</v>
-      </c>
-      <c r="Q18" t="s">
-        <v>102</v>
-      </c>
       <c r="R18" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="S18" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="Y18">
         <v>0.65</v>
       </c>
       <c r="AA18" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="AB18" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="19" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B19" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E19" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F19" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="I19" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="J19" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="M19" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="N19" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="Q19" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="R19" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="S19" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="Y19">
         <v>0.65</v>
       </c>
       <c r="AA19" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="AB19" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="20" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B20" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E20" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F20" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="I20" t="s">
+        <v>105</v>
+      </c>
+      <c r="J20" t="s">
+        <v>27</v>
+      </c>
+      <c r="L20" t="s">
+        <v>106</v>
+      </c>
+      <c r="M20" t="s">
+        <v>29</v>
+      </c>
+      <c r="N20" t="s">
         <v>107</v>
       </c>
-      <c r="J20" t="s">
-        <v>29</v>
-      </c>
-      <c r="L20" t="s">
+      <c r="Q20" t="s">
+        <v>100</v>
+      </c>
+      <c r="R20" t="s">
+        <v>36</v>
+      </c>
+      <c r="S20" t="s">
+        <v>101</v>
+      </c>
+      <c r="Y20">
+        <v>0.65</v>
+      </c>
+      <c r="AA20" t="s">
         <v>108</v>
       </c>
-      <c r="M20" t="s">
-        <v>31</v>
-      </c>
-      <c r="N20" t="s">
-        <v>109</v>
-      </c>
-      <c r="Q20" t="s">
-        <v>102</v>
-      </c>
-      <c r="R20" t="s">
-        <v>38</v>
-      </c>
-      <c r="S20" t="s">
-        <v>103</v>
-      </c>
-      <c r="Y20">
-        <v>0.65</v>
-      </c>
-      <c r="AA20" t="s">
-        <v>110</v>
-      </c>
       <c r="AB20" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="21" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B21" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E21" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F21" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="I21" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="J21" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="M21" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="N21" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="Q21" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="R21" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="S21" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="Y21">
         <v>0.65</v>
       </c>
       <c r="AA21" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="AB21" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="22" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
+        <v>111</v>
+      </c>
+      <c r="B22" t="s">
+        <v>32</v>
+      </c>
+      <c r="E22" t="s">
+        <v>33</v>
+      </c>
+      <c r="F22" t="s">
+        <v>112</v>
+      </c>
+      <c r="I22" t="s">
         <v>113</v>
       </c>
-      <c r="B22" t="s">
-        <v>34</v>
-      </c>
-      <c r="E22" t="s">
-        <v>35</v>
-      </c>
-      <c r="F22" t="s">
+      <c r="J22" t="s">
+        <v>32</v>
+      </c>
+      <c r="M22" t="s">
+        <v>33</v>
+      </c>
+      <c r="N22" t="s">
         <v>114</v>
       </c>
-      <c r="I22" t="s">
+      <c r="Q22" t="s">
+        <v>100</v>
+      </c>
+      <c r="R22" t="s">
+        <v>36</v>
+      </c>
+      <c r="S22" t="s">
+        <v>101</v>
+      </c>
+      <c r="Y22">
+        <v>0.65</v>
+      </c>
+      <c r="AA22" t="s">
         <v>115</v>
       </c>
-      <c r="J22" t="s">
-        <v>34</v>
-      </c>
-      <c r="M22" t="s">
-        <v>35</v>
-      </c>
-      <c r="N22" t="s">
-        <v>116</v>
-      </c>
-      <c r="Q22" t="s">
-        <v>102</v>
-      </c>
-      <c r="R22" t="s">
-        <v>38</v>
-      </c>
-      <c r="S22" t="s">
-        <v>103</v>
-      </c>
-      <c r="Y22">
-        <v>0.65</v>
-      </c>
-      <c r="AA22" t="s">
-        <v>117</v>
-      </c>
       <c r="AB22" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="23" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
+        <v>72</v>
+      </c>
+      <c r="B23" t="s">
+        <v>27</v>
+      </c>
+      <c r="D23" t="s">
+        <v>73</v>
+      </c>
+      <c r="E23" t="s">
+        <v>29</v>
+      </c>
+      <c r="F23" t="s">
         <v>74</v>
       </c>
-      <c r="B23" t="s">
-        <v>29</v>
-      </c>
-      <c r="D23" t="s">
-        <v>75</v>
-      </c>
-      <c r="E23" t="s">
-        <v>31</v>
-      </c>
-      <c r="F23" t="s">
-        <v>76</v>
-      </c>
       <c r="I23" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="J23" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="M23" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="N23" t="s">
+        <v>114</v>
+      </c>
+      <c r="Q23" t="s">
+        <v>100</v>
+      </c>
+      <c r="R23" t="s">
+        <v>36</v>
+      </c>
+      <c r="S23" t="s">
+        <v>101</v>
+      </c>
+      <c r="Y23">
+        <v>0.65</v>
+      </c>
+      <c r="AA23" t="s">
         <v>116</v>
       </c>
-      <c r="Q23" t="s">
-        <v>102</v>
-      </c>
-      <c r="R23" t="s">
-        <v>38</v>
-      </c>
-      <c r="S23" t="s">
-        <v>103</v>
-      </c>
-      <c r="Y23">
-        <v>0.65</v>
-      </c>
-      <c r="AA23" t="s">
-        <v>118</v>
-      </c>
       <c r="AB23" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="24" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B24" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E24" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F24" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="I24" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="J24" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="M24" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="N24" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="R24" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="S24" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="Y24">
         <v>0.65</v>
       </c>
       <c r="AA24" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="AB24" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="25" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B25" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E25" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F25" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="I25" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="J25" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="M25" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="N25" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="R25" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="S25" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="Y25">
         <v>0.65</v>
       </c>
       <c r="AA25" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="AB25" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="26" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
+        <v>120</v>
+      </c>
+      <c r="B26" t="s">
+        <v>27</v>
+      </c>
+      <c r="D26" t="s">
+        <v>121</v>
+      </c>
+      <c r="E26" t="s">
+        <v>29</v>
+      </c>
+      <c r="F26" t="s">
         <v>122</v>
       </c>
-      <c r="B26" t="s">
-        <v>29</v>
-      </c>
-      <c r="D26" t="s">
+      <c r="I26" t="s">
+        <v>92</v>
+      </c>
+      <c r="J26" t="s">
+        <v>27</v>
+      </c>
+      <c r="L26" t="s">
+        <v>93</v>
+      </c>
+      <c r="M26" t="s">
+        <v>29</v>
+      </c>
+      <c r="N26" t="s">
+        <v>94</v>
+      </c>
+      <c r="S26" t="s">
+        <v>117</v>
+      </c>
+      <c r="Y26">
+        <v>0.65</v>
+      </c>
+      <c r="AA26" t="s">
         <v>123</v>
       </c>
-      <c r="E26" t="s">
-        <v>31</v>
-      </c>
-      <c r="F26" t="s">
-        <v>124</v>
-      </c>
-      <c r="I26" t="s">
-        <v>94</v>
-      </c>
-      <c r="J26" t="s">
-        <v>29</v>
-      </c>
-      <c r="L26" t="s">
-        <v>95</v>
-      </c>
-      <c r="M26" t="s">
-        <v>31</v>
-      </c>
-      <c r="N26" t="s">
-        <v>96</v>
-      </c>
-      <c r="S26" t="s">
-        <v>119</v>
-      </c>
-      <c r="Y26">
-        <v>0.65</v>
-      </c>
-      <c r="AA26" t="s">
-        <v>125</v>
-      </c>
       <c r="AB26" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="27" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B27" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E27" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F27" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="I27" t="s">
+        <v>86</v>
+      </c>
+      <c r="J27" t="s">
+        <v>27</v>
+      </c>
+      <c r="L27" t="s">
+        <v>87</v>
+      </c>
+      <c r="M27" t="s">
+        <v>29</v>
+      </c>
+      <c r="N27" t="s">
         <v>88</v>
       </c>
-      <c r="J27" t="s">
-        <v>29</v>
-      </c>
-      <c r="L27" t="s">
+      <c r="R27" t="s">
+        <v>36</v>
+      </c>
+      <c r="S27" t="s">
+        <v>117</v>
+      </c>
+      <c r="Y27">
+        <v>0.65</v>
+      </c>
+      <c r="AA27" t="s">
         <v>89</v>
       </c>
-      <c r="M27" t="s">
-        <v>31</v>
-      </c>
-      <c r="N27" t="s">
-        <v>90</v>
-      </c>
-      <c r="R27" t="s">
-        <v>38</v>
-      </c>
-      <c r="S27" t="s">
-        <v>119</v>
-      </c>
-      <c r="Y27">
-        <v>0.65</v>
-      </c>
-      <c r="AA27" t="s">
-        <v>91</v>
-      </c>
       <c r="AB27" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="28" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B28" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E28" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F28" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="I28" t="s">
+        <v>92</v>
+      </c>
+      <c r="J28" t="s">
+        <v>27</v>
+      </c>
+      <c r="L28" t="s">
+        <v>93</v>
+      </c>
+      <c r="M28" t="s">
+        <v>29</v>
+      </c>
+      <c r="N28" t="s">
         <v>94</v>
       </c>
-      <c r="J28" t="s">
-        <v>29</v>
-      </c>
-      <c r="L28" t="s">
+      <c r="R28" t="s">
+        <v>36</v>
+      </c>
+      <c r="S28" t="s">
+        <v>117</v>
+      </c>
+      <c r="Y28">
+        <v>0.65</v>
+      </c>
+      <c r="AA28" t="s">
         <v>95</v>
       </c>
-      <c r="M28" t="s">
-        <v>31</v>
-      </c>
-      <c r="N28" t="s">
-        <v>96</v>
-      </c>
-      <c r="R28" t="s">
-        <v>38</v>
-      </c>
-      <c r="S28" t="s">
-        <v>119</v>
-      </c>
-      <c r="Y28">
-        <v>0.65</v>
-      </c>
-      <c r="AA28" t="s">
-        <v>97</v>
-      </c>
       <c r="AB28" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="29" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
+        <v>72</v>
+      </c>
+      <c r="B29" t="s">
+        <v>27</v>
+      </c>
+      <c r="D29" t="s">
+        <v>73</v>
+      </c>
+      <c r="E29" t="s">
+        <v>29</v>
+      </c>
+      <c r="F29" t="s">
         <v>74</v>
       </c>
-      <c r="B29" t="s">
-        <v>29</v>
-      </c>
-      <c r="D29" t="s">
-        <v>75</v>
-      </c>
-      <c r="E29" t="s">
-        <v>31</v>
-      </c>
-      <c r="F29" t="s">
-        <v>76</v>
-      </c>
       <c r="I29" t="s">
+        <v>57</v>
+      </c>
+      <c r="J29" t="s">
+        <v>27</v>
+      </c>
+      <c r="L29" t="s">
+        <v>58</v>
+      </c>
+      <c r="M29" t="s">
+        <v>29</v>
+      </c>
+      <c r="N29" t="s">
         <v>59</v>
       </c>
-      <c r="J29" t="s">
-        <v>29</v>
-      </c>
-      <c r="L29" t="s">
-        <v>60</v>
-      </c>
-      <c r="M29" t="s">
-        <v>31</v>
-      </c>
-      <c r="N29" t="s">
-        <v>61</v>
-      </c>
       <c r="S29" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="Y29">
         <v>0.98921999999999999</v>
       </c>
       <c r="AA29" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="AB29" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="30" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
+        <v>72</v>
+      </c>
+      <c r="B30" t="s">
+        <v>27</v>
+      </c>
+      <c r="D30" t="s">
+        <v>73</v>
+      </c>
+      <c r="E30" t="s">
+        <v>29</v>
+      </c>
+      <c r="F30" t="s">
         <v>74</v>
       </c>
-      <c r="B30" t="s">
-        <v>29</v>
-      </c>
-      <c r="D30" t="s">
-        <v>75</v>
-      </c>
-      <c r="E30" t="s">
-        <v>31</v>
-      </c>
-      <c r="F30" t="s">
-        <v>76</v>
-      </c>
       <c r="I30" t="s">
+        <v>128</v>
+      </c>
+      <c r="J30" t="s">
+        <v>27</v>
+      </c>
+      <c r="L30" t="s">
+        <v>129</v>
+      </c>
+      <c r="M30" t="s">
+        <v>29</v>
+      </c>
+      <c r="N30" t="s">
         <v>130</v>
       </c>
-      <c r="J30" t="s">
-        <v>29</v>
-      </c>
-      <c r="L30" t="s">
-        <v>131</v>
-      </c>
-      <c r="M30" t="s">
-        <v>31</v>
-      </c>
-      <c r="N30" t="s">
-        <v>132</v>
-      </c>
       <c r="S30" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="Y30">
         <v>0.98921999999999999</v>
       </c>
       <c r="AA30" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="AB30" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="31" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
+        <v>72</v>
+      </c>
+      <c r="B31" t="s">
+        <v>27</v>
+      </c>
+      <c r="D31" t="s">
+        <v>73</v>
+      </c>
+      <c r="E31" t="s">
+        <v>29</v>
+      </c>
+      <c r="F31" t="s">
         <v>74</v>
       </c>
-      <c r="B31" t="s">
-        <v>29</v>
-      </c>
-      <c r="D31" t="s">
-        <v>75</v>
-      </c>
-      <c r="E31" t="s">
-        <v>31</v>
-      </c>
-      <c r="F31" t="s">
-        <v>76</v>
-      </c>
       <c r="I31" t="s">
+        <v>132</v>
+      </c>
+      <c r="J31" t="s">
+        <v>27</v>
+      </c>
+      <c r="L31" t="s">
+        <v>133</v>
+      </c>
+      <c r="M31" t="s">
+        <v>29</v>
+      </c>
+      <c r="N31" t="s">
         <v>134</v>
       </c>
-      <c r="J31" t="s">
-        <v>29</v>
-      </c>
-      <c r="L31" t="s">
-        <v>135</v>
-      </c>
-      <c r="M31" t="s">
-        <v>31</v>
-      </c>
-      <c r="N31" t="s">
-        <v>136</v>
-      </c>
       <c r="S31" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="Y31">
         <v>0.98040000000000005</v>
       </c>
       <c r="AA31" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="AB31" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>

</xml_diff>